<commit_message>
added leet code two sums problem
</commit_message>
<xml_diff>
--- a/abbott_milk_formulas.xlsx
+++ b/abbott_milk_formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yeshwanth\Desktop\uyyaala to kidsfud products\milk_formulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB8D3EC-F519-4BC7-90BE-F32C960D5220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A73A5E-6882-4343-BE2A-665330B28E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>https://www.uyyaala.com/products/abbott-similac-gold-stage-1-new-advanced-milk-formula-with-hmo-400g-0-6m</t>
   </si>
@@ -37,9 +37,6 @@
     <t>https://www.uyyaala.com/products/abbott-pediasure-complete-and-balance-nutrition-vanilla-1-10-years-400-gmimported</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-step-1-milk-based-infant-formula-0-months-850g</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-similac-advance-2-after-6-months</t>
   </si>
   <si>
@@ -67,103 +64,49 @@
     <t>https://www.uyyaala.com/products/abbott-similac-iq-follow-up-formula-stage-3-12-to-24-months-400g</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-iq-follow-up-formula-stage-2-6-to-12-months-400g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-pro-advance-infant-formula-with-2-fl-hmo-for-immune-support-non-gmo-baby-formula-powder-964g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-advance-infant-formula-for-brain-immunity-development-stage-1-up-to-6-months-400g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-advance-3-12-to-24-months</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-pediasure-complete-triple-sure-honey-1-10-years-400g-imported</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-milk-formula-0-to-24months-350gms</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-pro-sensitive-infant-formula-with-2-fl-hmo-for-immune-support-non-gmo-baby-formula-964-gms</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/similac-360-total-care-infant-milk-formula-1-13kg</t>
   </si>
   <si>
     <t>https://www.uyyaala.com/products/similac-sensitive-360-total-care-infant-milk-formula-1-13kg</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-stage-3-follow-up-formula-from-12-to-24-months-400g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-formula-360g-stage-3-from-1-to-3-years-imported</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-advance-infant-formula-for-brain-immunity-development-stage-1-up-to-6-months-200g-jar</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-advance-optigro-complete-nutrition-infant-formula-for-0-12-months-1-13-kg</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-step-1-lower-iron-non-gmo-milk-based-infant-formula-0-months-850g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-go-grow-toddler-drink-milk-based-powder-850g-12-36m</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-formula-350g-stage-2-from-6-to-12-months-imported</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-sensitive-infant-formula-for-fussiness-gas-due-to-lactose-sensitivity-1-13kg</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-pro-advance-infant-formula-with-2-fl-hmo-for-immune-support-non-gmo-baby-formula-powder-873g-tin-pack</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-gold-infant-milk-formula-stage-1-360gms-0-6months-imported</t>
   </si>
   <si>
     <t>https://www.uyyaala.com/products/abbott-similac-follow-up-formula-stage-4-18-to-24-months-400g</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-go-grow-toddler-drink-milk-based-powder-873g-12-36m</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-go-grow-sensitive-toddler-drink-for-lactose-sensitivity-661g-12-36m</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-chocolate-flavour-2-years-1kg</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-kesar-badam-flavour-2-years-200-g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-similac-advance-4-infant-formula-from-18-to-24m-400g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/similac-pro-advance-infant-formula-with-2-fl-hmo-for-immune-support-non-gmo-baby-formula-powder-584g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-vanilla-delight-flavour-2-years-400-g-jar</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-chocolate-flavour-2-years-400-g-jar</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-with-chocolate-delight-flavour-for-2-years-750g</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-chocolate-flavour-2-years-200-g-jar</t>
   </si>
   <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-chocolate-flavour-2-years-400-g</t>
-  </si>
-  <si>
-    <t>https://www.uyyaala.com/products/abbott-pediasure-vanilla-delite-flavour-2-years-750g</t>
-  </si>
-  <si>
     <t>https://www.uyyaala.com/products/abbott-pediasure-vanilla-delight-flavour-2years</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-vanilla-delight-flavour-2-years-200-g</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-vanilla-delight-flavour-2-years-400-g</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-pediasure-complete-balanced-nutrition-to-help-kids-grow-box-nutrition-drink-refill-pack-chocolate-flavour-2-years-200-g</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-milk-formula-0-to-6months-350gms</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-formula-360g-stage-2-from-6-12-months-imported</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/abbott-similac-total-comfort-infant-formula-360g-stage-3-from-1-3-years-imported</t>
+  </si>
+  <si>
+    <t>https://www.uyyaala.com/products/similac-advance-optigro-complete-nutrition-infant-formula-for-0-12-months-352gms</t>
   </si>
   <si>
     <t>urls</t>
@@ -529,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -539,7 +482,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,158 +715,6 @@
       </c>
       <c r="B30" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>